<commit_message>
Changed Header without special characters
</commit_message>
<xml_diff>
--- a/Domain/Results/Benchmarks/GenerateInitialPopulation_Results.xlsx
+++ b/Domain/Results/Benchmarks/GenerateInitialPopulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\source\repos\QAP\Domain\Results\Benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4619DF0-7AD9-4770-B521-2609FB6D27F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10F2D46-8B75-4572-A0A3-6A68D4807892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{6A217BFE-ADC4-461B-BFD6-8651FE474739}"/>
   </bookViews>
@@ -82,9 +82,6 @@
     <t>NrOfSolutions</t>
   </si>
   <si>
-    <t>Mean</t>
-  </si>
-  <si>
     <t>Error[us]</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
   </si>
   <si>
     <t>Gen1</t>
-  </si>
-  <si>
-    <t>Allocated[B]</t>
   </si>
   <si>
     <t>StepWisePopulationGeneration</t>
@@ -170,6 +164,12 @@
   </si>
   <si>
     <t>3.9063</t>
+  </si>
+  <si>
+    <t>MeanUs</t>
+  </si>
+  <si>
+    <t>AllocatedB</t>
   </si>
 </sst>
 </file>
@@ -263,13 +263,13 @@
     <tableColumn id="1" xr3:uid="{006B30B1-427A-4EED-ABD6-54B950C4F8C8}" uniqueName="1" name="Method" queryTableFieldId="1" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{8497C9EA-73A0-4DB0-A1D0-8758F9D0233C}" uniqueName="2" name="SolutionName" queryTableFieldId="2" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{61CBFB74-8EE8-403B-8CA3-2F8596BD6A2A}" uniqueName="3" name="NrOfSolutions" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{370033FE-8313-4DCC-973D-3763BC1AA781}" uniqueName="4" name="Mean" queryTableFieldId="4"/>
+    <tableColumn id="4" xr3:uid="{370033FE-8313-4DCC-973D-3763BC1AA781}" uniqueName="4" name="MeanUs" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{F95C0237-C8D6-4492-89C9-B9EF0E0162FA}" uniqueName="5" name="Error[us]" queryTableFieldId="5"/>
     <tableColumn id="6" xr3:uid="{FC01C39A-F40B-4535-9B2E-AB051B6D76B4}" uniqueName="6" name="StdDev[us]" queryTableFieldId="6"/>
     <tableColumn id="7" xr3:uid="{073BA56B-3BD3-4E8F-A500-9E78331FAAA3}" uniqueName="7" name="Median[us]" queryTableFieldId="7"/>
     <tableColumn id="8" xr3:uid="{22E612D5-7EEF-417E-B20E-BE9136C9F33F}" uniqueName="8" name="Gen0" queryTableFieldId="8" dataDxfId="1"/>
     <tableColumn id="9" xr3:uid="{61747C82-68E8-4B0D-8444-46202F8EBE74}" uniqueName="9" name="Gen1" queryTableFieldId="9" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{6D960E74-92A6-4E16-AC53-659785D0A773}" uniqueName="10" name="Allocated[B]" queryTableFieldId="10"/>
+    <tableColumn id="10" xr3:uid="{6D960E74-92A6-4E16-AC53-659785D0A773}" uniqueName="10" name="AllocatedB" queryTableFieldId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -575,7 +575,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,33 +602,33 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -646,10 +646,10 @@
         <v>4.8109999999999999</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J2">
         <v>1016</v>
@@ -657,10 +657,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -678,10 +678,10 @@
         <v>7.5529999999999999</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J3">
         <v>1016</v>
@@ -689,10 +689,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -710,10 +710,10 @@
         <v>8.7579999999999991</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J4">
         <v>5809</v>
@@ -721,10 +721,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -742,10 +742,10 @@
         <v>49.377000000000002</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J5">
         <v>9656</v>
@@ -753,10 +753,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -774,10 +774,10 @@
         <v>73.683000000000007</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J6">
         <v>9656</v>
@@ -785,10 +785,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>100</v>
@@ -806,10 +806,10 @@
         <v>77.162999999999997</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J7">
         <v>53462</v>
@@ -817,10 +817,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>200</v>
@@ -838,10 +838,10 @@
         <v>98.07</v>
       </c>
       <c r="H8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J8">
         <v>19256</v>
@@ -849,10 +849,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>200</v>
@@ -870,10 +870,10 @@
         <v>147.416</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J9">
         <v>19256</v>
@@ -881,10 +881,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>200</v>
@@ -902,10 +902,10 @@
         <v>148.19200000000001</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J10">
         <v>106539</v>
@@ -913,10 +913,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -934,10 +934,10 @@
         <v>14.728</v>
       </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J11">
         <v>1576</v>
@@ -945,10 +945,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -966,10 +966,10 @@
         <v>20.09</v>
       </c>
       <c r="H12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J12">
         <v>1576</v>
@@ -977,10 +977,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -998,10 +998,10 @@
         <v>20.045000000000002</v>
       </c>
       <c r="H13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J13">
         <v>7951</v>
@@ -1009,10 +1009,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>100</v>
@@ -1030,10 +1030,10 @@
         <v>147.126</v>
       </c>
       <c r="H14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J14">
         <v>15256</v>
@@ -1041,10 +1041,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15">
         <v>100</v>
@@ -1062,10 +1062,10 @@
         <v>205.858</v>
       </c>
       <c r="H15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J15">
         <v>15256</v>
@@ -1073,10 +1073,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>100</v>
@@ -1094,10 +1094,10 @@
         <v>133.66300000000001</v>
       </c>
       <c r="H16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J16">
         <v>74297</v>
@@ -1105,10 +1105,10 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17">
         <v>200</v>
@@ -1126,10 +1126,10 @@
         <v>290.916</v>
       </c>
       <c r="H17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J17">
         <v>30456</v>
@@ -1137,10 +1137,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18">
         <v>200</v>
@@ -1158,10 +1158,10 @@
         <v>396.66800000000001</v>
       </c>
       <c r="H18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J18">
         <v>30456</v>
@@ -1169,10 +1169,10 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>200</v>
@@ -1190,10 +1190,10 @@
         <v>249.83500000000001</v>
       </c>
       <c r="H19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J19">
         <v>148140</v>
@@ -1201,10 +1201,10 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20">
         <v>10</v>
@@ -1222,10 +1222,10 @@
         <v>1029.769</v>
       </c>
       <c r="H20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J20">
         <v>10778</v>
@@ -1233,10 +1233,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C21">
         <v>10</v>
@@ -1254,10 +1254,10 @@
         <v>1114.568</v>
       </c>
       <c r="H21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J21">
         <v>10778</v>
@@ -1265,10 +1265,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C22">
         <v>10</v>
@@ -1286,10 +1286,10 @@
         <v>283.108</v>
       </c>
       <c r="H22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J22">
         <v>35793</v>
@@ -1297,10 +1297,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C23">
         <v>100</v>
@@ -1318,10 +1318,10 @@
         <v>10118.733</v>
       </c>
       <c r="H23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J23">
         <v>107274</v>
@@ -1329,10 +1329,10 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C24">
         <v>100</v>
@@ -1350,10 +1350,10 @@
         <v>11087.424999999999</v>
       </c>
       <c r="H24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J24">
         <v>107274</v>
@@ -1361,10 +1361,10 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25">
         <v>100</v>
@@ -1382,10 +1382,10 @@
         <v>1717.8309999999999</v>
       </c>
       <c r="H25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I25" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J25">
         <v>352706</v>
@@ -1393,10 +1393,10 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C26">
         <v>200</v>
@@ -1414,10 +1414,10 @@
         <v>20457.330999999998</v>
       </c>
       <c r="H26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J26">
         <v>214491</v>
@@ -1425,10 +1425,10 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C27">
         <v>200</v>
@@ -1446,10 +1446,10 @@
         <v>22084.953000000001</v>
       </c>
       <c r="H27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J27">
         <v>214493</v>
@@ -1457,10 +1457,10 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C28">
         <v>200</v>
@@ -1478,10 +1478,10 @@
         <v>3261.2710000000002</v>
       </c>
       <c r="H28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J28">
         <v>704948</v>
@@ -1500,7 +1500,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D28"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1524,7 +1524,7 @@
         <v>NrOfSolutions</v>
       </c>
       <c r="D1" t="str">
-        <v>Mean</v>
+        <v>MeanUs</v>
       </c>
       <c r="E1" t="str">
         <v>Error[us]</v>
@@ -1542,7 +1542,7 @@
         <v>Gen1</v>
       </c>
       <c r="J1" t="str">
-        <v>Allocated[B]</v>
+        <v>AllocatedB</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2420,7 +2420,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2443,7 +2443,7 @@
         <v>NrOfSolutions</v>
       </c>
       <c r="D1" t="str">
-        <v>Mean</v>
+        <v>MeanUs</v>
       </c>
       <c r="E1" t="str">
         <v>Error[us]</v>
@@ -2461,7 +2461,7 @@
         <v>Gen1</v>
       </c>
       <c r="J1" t="str">
-        <v>Allocated[B]</v>
+        <v>AllocatedB</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>